<commit_message>
Static vs. Dynamic Properties.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/doc/evolution/StaticPropertyUUIDGeneration_Proposal/STATIC_PROPERTY_UUIDS_REGULATED.xlsx
+++ b/docs/src/main/asciidoc/dist/doc/evolution/StaticPropertyUUIDGeneration_Proposal/STATIC_PROPERTY_UUIDS_REGULATED.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12840" tabRatio="588" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12840" tabRatio="588"/>
   </bookViews>
   <sheets>
     <sheet name="SC-References" sheetId="16" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="37" r:id="rId2"/>
+    <sheet name="EG-Convictions" sheetId="37" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="126">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -337,9 +337,6 @@
     <t>42119227bf1a9081775218c4f1ae36d9</t>
   </si>
   <si>
-    <t>Apparent collision</t>
-  </si>
-  <si>
     <t>ACME, Ltd.</t>
   </si>
   <si>
@@ -389,6 +386,18 @@
   </si>
   <si>
     <t>008732cf68215d1fa6c4f0a33349cdca</t>
+  </si>
+  <si>
+    <t>Accused of participation in a group for collision purposes</t>
+  </si>
+  <si>
+    <t>Accused of belonging to the Italian Mafia</t>
+  </si>
+  <si>
+    <t>Two years</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -925,7 +934,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1005,6 +1014,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1355,9 +1367,7 @@
   <sheetPr codeName="Hoja20"/>
   <dimension ref="A1:Z60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3771,7 +3781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -4168,7 +4178,7 @@
         <v>0</v>
       </c>
       <c r="U7" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="V7" s="6" t="s">
         <v>0</v>
@@ -4271,7 +4281,7 @@
         <v>26</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="U9" s="12">
         <v>1</v>
@@ -4325,7 +4335,7 @@
         <v>28</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U10" s="12">
         <v>1</v>
@@ -4379,7 +4389,7 @@
         <v>29</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U11" s="12">
         <v>1</v>
@@ -4486,8 +4496,8 @@
       <c r="S13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="T13" s="4" t="b">
-        <v>0</v>
+      <c r="T13" s="30" t="s">
+        <v>125</v>
       </c>
       <c r="U13" s="12">
         <v>1</v>
@@ -4599,7 +4609,7 @@
         <v>33</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U15" s="12">
         <v>1</v>
@@ -4810,7 +4820,7 @@
         <v>0</v>
       </c>
       <c r="U19" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V19" s="6" t="s">
         <v>0</v>
@@ -4858,8 +4868,8 @@
       <c r="S20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="T20" s="8" t="s">
-        <v>47</v>
+      <c r="T20" s="8">
+        <v>42430</v>
       </c>
       <c r="U20" s="12">
         <v>1</v>
@@ -4868,10 +4878,10 @@
         <v>25</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X20" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Y20" s="6" t="s">
         <v>0</v>
@@ -4913,7 +4923,7 @@
         <v>26</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="U21" s="12">
         <v>1</v>
@@ -4922,10 +4932,10 @@
         <v>27</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X21" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Y21" s="6" t="s">
         <v>0</v>
@@ -4967,7 +4977,7 @@
         <v>28</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U22" s="12">
         <v>1</v>
@@ -4976,10 +4986,10 @@
         <v>27</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X22" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y22" s="6" t="s">
         <v>0</v>
@@ -5021,7 +5031,7 @@
         <v>29</v>
       </c>
       <c r="T23" s="8" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="U23" s="12">
         <v>1</v>
@@ -5030,10 +5040,10 @@
         <v>27</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="X23" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y23" s="6" t="s">
         <v>0</v>
@@ -5128,8 +5138,8 @@
       <c r="S25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="T25" s="4" t="b">
-        <v>0</v>
+      <c r="T25" s="30" t="s">
+        <v>125</v>
       </c>
       <c r="U25" s="12">
         <v>1</v>
@@ -5138,10 +5148,10 @@
         <v>16</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="X25" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Y25" s="4" t="s">
         <v>0</v>
@@ -5241,7 +5251,7 @@
         <v>33</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U27" s="12">
         <v>1</v>
@@ -5250,10 +5260,10 @@
         <v>27</v>
       </c>
       <c r="W27" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="X27" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="X27" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="Y27" s="4" t="s">
         <v>0</v>

</xml_diff>